<commit_message>
calculated avg transfer time
</commit_message>
<xml_diff>
--- a/ampl/results/Result_Analysis.xlsx
+++ b/ampl/results/Result_Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="6660" yWindow="0" windowWidth="18680" windowHeight="13400" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="11940" yWindow="480" windowWidth="18680" windowHeight="13400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Saturday Morning" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="47">
   <si>
     <t>Time to Station</t>
   </si>
@@ -149,13 +149,25 @@
   </si>
   <si>
     <t>Orange</t>
+  </si>
+  <si>
+    <t>Saturday Evening</t>
+  </si>
+  <si>
+    <t>Objective Function</t>
+  </si>
+  <si>
+    <t>Total Transfers</t>
+  </si>
+  <si>
+    <t>Avg Transfer Wait Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -191,6 +203,14 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -209,22 +229,43 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -556,8 +597,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1233,6 +1274,12 @@
       <c r="B24">
         <v>10</v>
       </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
@@ -1241,6 +1288,13 @@
       <c r="B25">
         <v>3</v>
       </c>
+      <c r="D25" s="2">
+        <v>47517.25</v>
+      </c>
+      <c r="F25">
+        <f>D28/D25</f>
+        <v>1.3172374243038054</v>
+      </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
@@ -1257,6 +1311,9 @@
       <c r="B27">
         <v>9</v>
       </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
@@ -1264,6 +1321,9 @@
       </c>
       <c r="B28">
         <v>3</v>
+      </c>
+      <c r="D28">
+        <v>62591.5</v>
       </c>
     </row>
     <row r="29" spans="1:12">
@@ -1292,8 +1352,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1716,7 +1776,7 @@
     </row>
     <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:10">
@@ -1969,6 +2029,12 @@
       <c r="B24">
         <v>11</v>
       </c>
+      <c r="D24" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="25" spans="1:12">
       <c r="A25" t="s">
@@ -1977,6 +2043,13 @@
       <c r="B25">
         <v>5</v>
       </c>
+      <c r="D25" s="2">
+        <v>43878</v>
+      </c>
+      <c r="F25">
+        <f>D28/D25</f>
+        <v>2.6778396918729204</v>
+      </c>
     </row>
     <row r="26" spans="1:12">
       <c r="A26" t="s">
@@ -1993,6 +2066,9 @@
       <c r="B27">
         <v>10</v>
       </c>
+      <c r="D27" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="28" spans="1:12">
       <c r="A28" t="s">
@@ -2000,6 +2076,9 @@
       </c>
       <c r="B28">
         <v>4</v>
+      </c>
+      <c r="D28">
+        <v>117498.25</v>
       </c>
     </row>
     <row r="29" spans="1:12">

</xml_diff>

<commit_message>
removed old versions of formulation
</commit_message>
<xml_diff>
--- a/ampl/results/Result_Analysis.xlsx
+++ b/ampl/results/Result_Analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="11940" yWindow="480" windowWidth="18680" windowHeight="13400" tabRatio="500"/>
+    <workbookView xWindow="9820" yWindow="620" windowWidth="18680" windowHeight="13400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Saturday Morning" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="49">
   <si>
     <t>Time to Station</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>Avg Transfer Wait Time</t>
+  </si>
+  <si>
+    <t>Base Objective Function</t>
+  </si>
+  <si>
+    <t>Base Avg Transfer Wait Time</t>
   </si>
 </sst>
 </file>
@@ -229,8 +235,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -251,7 +261,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="19">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -259,6 +269,8 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -266,6 +278,8 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -595,10 +609,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1332,6 +1346,23 @@
       </c>
       <c r="B29">
         <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="D30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="D31">
+        <v>256520</v>
+      </c>
+      <c r="F31">
+        <f>D31/D25</f>
+        <v>5.3984605590601307</v>
       </c>
     </row>
   </sheetData>
@@ -1350,10 +1381,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2087,6 +2118,23 @@
       </c>
       <c r="B29">
         <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="D30" t="s">
+        <v>47</v>
+      </c>
+      <c r="F30" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="D31">
+        <v>228052</v>
+      </c>
+      <c r="F31">
+        <f>D31/D25</f>
+        <v>5.1974110032362457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>